<commit_message>
remove duplicate records for today all
</commit_message>
<xml_diff>
--- a/risk_management/portfolio.xlsx
+++ b/risk_management/portfolio.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huiyang/Documents/quantest/risk_management/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{88D93CC0-274B-274D-B15D-A011F013DC49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18520" windowHeight="11000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -109,37 +103,40 @@
     <t>2018-03-16</t>
   </si>
   <si>
-    <t>7.628%</t>
-  </si>
-  <si>
-    <t>9.766%</t>
-  </si>
-  <si>
-    <t>13.387%</t>
-  </si>
-  <si>
-    <t>6.554%</t>
-  </si>
-  <si>
-    <t>6.213%</t>
+    <t>10.3%</t>
+  </si>
+  <si>
+    <t>8.683%</t>
+  </si>
+  <si>
+    <t>13.69%</t>
+  </si>
+  <si>
+    <t>7.344%</t>
+  </si>
+  <si>
+    <t>6.226%</t>
   </si>
   <si>
     <t>18.379%</t>
   </si>
   <si>
-    <t>-1.536%</t>
-  </si>
-  <si>
-    <t>2.603%</t>
-  </si>
-  <si>
-    <t>-1.269%</t>
-  </si>
-  <si>
-    <t>-4.028%</t>
+    <t>-15.479%</t>
+  </si>
+  <si>
+    <t>6.182%</t>
+  </si>
+  <si>
+    <t>-6.642%</t>
+  </si>
+  <si>
+    <t>-10.566%</t>
   </si>
   <si>
     <t>-0.739%</t>
+  </si>
+  <si>
+    <t>2018-03-23</t>
   </si>
   <si>
     <t>N</t>
@@ -151,12 +148,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -164,15 +161,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -222,14 +212,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -276,7 +258,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,27 +290,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,24 +324,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,14 +499,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
@@ -623,7 +567,7 @@
         <v>25</v>
       </c>
       <c r="E2">
-        <v>12.856999999999999</v>
+        <v>12.857</v>
       </c>
       <c r="F2">
         <v>500</v>
@@ -650,7 +594,7 @@
         <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -673,28 +617,28 @@
         <v>2100</v>
       </c>
       <c r="I3">
-        <v>12.5</v>
+        <v>10.73</v>
       </c>
       <c r="J3">
         <v>12.98</v>
       </c>
       <c r="K3">
-        <v>11.99</v>
+        <v>11.643</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
       </c>
       <c r="M3">
-        <v>-409.5</v>
+        <v>-4126.5</v>
       </c>
       <c r="N3" t="s">
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -711,34 +655,34 @@
         <v>27</v>
       </c>
       <c r="E4">
-        <v>9.2200000000000006</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="F4">
         <v>500</v>
       </c>
       <c r="I4">
-        <v>9.4600000000000009</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="J4">
-        <v>9.7799999999999994</v>
+        <v>10.5</v>
       </c>
       <c r="K4">
-        <v>8.8249999999999993</v>
+        <v>9.587999999999999</v>
       </c>
       <c r="L4" t="s">
         <v>30</v>
       </c>
       <c r="M4">
-        <v>120</v>
+        <v>285</v>
       </c>
       <c r="N4" t="s">
         <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -761,28 +705,28 @@
         <v>400</v>
       </c>
       <c r="I5">
-        <v>12.68</v>
+        <v>11.99</v>
       </c>
       <c r="J5">
-        <v>13.26</v>
+        <v>13.55</v>
       </c>
       <c r="K5">
-        <v>11.484999999999999</v>
+        <v>11.695</v>
       </c>
       <c r="L5" t="s">
         <v>31</v>
       </c>
       <c r="M5">
-        <v>-65.2</v>
+        <v>-341.2</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -799,34 +743,34 @@
         <v>28</v>
       </c>
       <c r="E6">
-        <v>16.213000000000001</v>
+        <v>16.213</v>
       </c>
       <c r="F6">
         <v>400</v>
       </c>
       <c r="I6">
-        <v>15.56</v>
+        <v>14.5</v>
       </c>
       <c r="J6">
         <v>16.45</v>
       </c>
       <c r="K6">
-        <v>15.372</v>
+        <v>15.242</v>
       </c>
       <c r="L6" t="s">
         <v>32</v>
       </c>
       <c r="M6">
-        <v>-261.2</v>
+        <v>-685.2</v>
       </c>
       <c r="N6" t="s">
         <v>38</v>
       </c>
       <c r="O6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="P6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -843,7 +787,7 @@
         <v>28</v>
       </c>
       <c r="E7">
-        <v>17.196999999999999</v>
+        <v>17.197</v>
       </c>
       <c r="F7">
         <v>300</v>
@@ -855,7 +799,7 @@
         <v>15.45</v>
       </c>
       <c r="K7">
-        <v>14.49</v>
+        <v>14.488</v>
       </c>
       <c r="L7" t="s">
         <v>33</v>
@@ -867,15 +811,13 @@
         <v>39</v>
       </c>
       <c r="O7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update for factor analysis
</commit_message>
<xml_diff>
--- a/risk_management/portfolio.xlsx
+++ b/risk_management/portfolio.xlsx
@@ -682,7 +682,7 @@
         <v>40</v>
       </c>
       <c r="P4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -726,7 +726,7 @@
         <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16">

</xml_diff>